<commit_message>
Finished labeling 15 games, updated summaries
</commit_message>
<xml_diff>
--- a/static/data/notes/CandidateSummaries.xlsx
+++ b/static/data/notes/CandidateSummaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanos\Documents\Dev\NBAThesis\NBA_Thesis\static\data\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C622D82-F654-459B-9358-E22827ED9B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEA54BE-8B4A-49AB-8B2B-0D88C5FA429D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26192" yWindow="-1603" windowWidth="26301" windowHeight="14305" firstSheet="5" activeTab="6" xr2:uid="{62BF07D9-DBFF-4528-A9A8-7318055715EB}"/>
+    <workbookView xWindow="-26192" yWindow="-1603" windowWidth="26301" windowHeight="14305" xr2:uid="{62BF07D9-DBFF-4528-A9A8-7318055715EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,11 @@
     <sheet name="20151230LALBOS" sheetId="10" r:id="rId9"/>
     <sheet name="20151231PHXOKC" sheetId="6" r:id="rId10"/>
     <sheet name="20160102BKLBOS" sheetId="11" r:id="rId11"/>
-    <sheet name="20160113MIALAC" sheetId="12" r:id="rId12"/>
-    <sheet name="20160115DALCHI" sheetId="13" r:id="rId13"/>
-    <sheet name="20160115MINOKC" sheetId="14" r:id="rId14"/>
-    <sheet name="20160118PHINYK" sheetId="16" r:id="rId15"/>
-    <sheet name="20160120MIAWAS" sheetId="18" r:id="rId16"/>
-    <sheet name="20160123LALPOR" sheetId="15" r:id="rId17"/>
+    <sheet name="20160115DALCHI" sheetId="13" r:id="rId12"/>
+    <sheet name="20160115MINOKC" sheetId="14" r:id="rId13"/>
+    <sheet name="20160118PHINYK" sheetId="16" r:id="rId14"/>
+    <sheet name="20160120MIAWAS" sheetId="18" r:id="rId15"/>
+    <sheet name="20160123LALPOR" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="38">
   <si>
     <t>positive candidates</t>
   </si>
@@ -149,6 +148,21 @@
   </si>
   <si>
     <t>Players all mixed up</t>
+  </si>
+  <si>
+    <t>backdoor pass follows</t>
+  </si>
+  <si>
+    <t>screener very far from cutter</t>
+  </si>
+  <si>
+    <t>borderline, far from screen, shoots right away</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>missing game tape for last 3/4 of 4th quarter</t>
   </si>
 </sst>
 </file>
@@ -560,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C99D260-17EE-4B29-B6BB-D4F26CA46663}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -582,7 +596,7 @@
       </c>
       <c r="B2">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B2)</f>
-        <v>711</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -591,7 +605,7 @@
       </c>
       <c r="B3">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B3)</f>
-        <v>1437</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -600,7 +614,7 @@
       </c>
       <c r="B4">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B4)</f>
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -609,7 +623,7 @@
       </c>
       <c r="B5">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B5)</f>
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,8 +631,8 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <f>AVERAGE('20151106MILNYK:20160123LALPOR'!B6)</f>
-        <v>0.9027670990040001</v>
+        <f>(B2 - B4)/(B2 - B4 + B5)</f>
+        <v>0.88309636650868883</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +645,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -791,485 +805,587 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2FF00F-24CF-47EB-A5FB-1C06B8AE7E0D}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="10.125" customWidth="1"/>
+    <col min="16" max="16" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.15833333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.92156862745098034</v>
+        <v>0.97142857142857142</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8.819444444444445E-2</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AFDDD1-ED78-44A8-B696-DE9D5F9BFE5D}">
-  <dimension ref="A1:O6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAA13AA-C891-4499-886B-F49D53CE49D8}">
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="10.125" customWidth="1"/>
+    <col min="16" max="16" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.92156862745098034</v>
+        <v>0.84</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5.347222222222222E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.47986111111111113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.31666666666666665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.36388888888888887</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.13541666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAA13AA-C891-4499-886B-F49D53CE49D8}">
-  <dimension ref="A1:O6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D75E1A-7ACE-40A0-9FEE-1575DE083FBC}">
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="10.125" customWidth="1"/>
+    <col min="16" max="16" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.27986111111111112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.22847222222222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.22569444444444445</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.92156862745098034</v>
+        <v>0.87878787878787878</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.44722222222222219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.14027777777777778</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D75E1A-7ACE-40A0-9FEE-1575DE083FBC}">
-  <dimension ref="A1:O6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="10.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.92156862745098034</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:L1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438F9ED1-D7F3-474D-8234-1A7404ACC185}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
@@ -1573,7 +1689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418834EC-AFF0-4E5D-A9B7-EF49AB1767E2}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
@@ -1931,7 +2047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D9984E-67ED-40E7-B805-C03D77494EDF}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
@@ -2279,7 +2395,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2469,9 +2585,9 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
-        <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.96296296296296291</v>
+      <c r="B6" s="7" t="b">
+        <f>Overall!B6=(B2 - B4)/(B2 - B4 + B5)</f>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>345</v>
@@ -2538,7 +2654,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3381,7 +3497,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="A1:XFD1048576"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3607,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065A868-8FBB-4D38-872A-E4D2D60D3BF7}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3978,7 +4094,215 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80036B7F-4E80-402C-9296-40787A3B819F}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="16" max="16" width="10.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>88</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.4680555555555555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.33819444444444446</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <f>(B2 - B4)/(B2 - B4 + B5)</f>
+        <v>0.86842105263157898</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.12083333333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.36319444444444443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.17708333333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA21A451-193D-4E3D-87E8-873BE8862B2B}">
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -3988,229 +4312,215 @@
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="10.125" customWidth="1"/>
+    <col min="16" max="16" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.32083333333333336</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.92156862745098034</v>
+        <v>0.9</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.44236111111111115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.23402777777777781</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.13541666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.44236111111111115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.17222222222222225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.23124999999999998</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:L1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA21A451-193D-4E3D-87E8-873BE8862B2B}">
-  <dimension ref="A1:O6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="10.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.92156862745098034</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding 15th game labled data
</commit_message>
<xml_diff>
--- a/static/data/notes/CandidateSummaries.xlsx
+++ b/static/data/notes/CandidateSummaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanos\Documents\Dev\NBAThesis\NBA_Thesis\static\data\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEA54BE-8B4A-49AB-8B2B-0D88C5FA429D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406D7350-7AC6-4D75-AF5D-4FD1FB0D2034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26192" yWindow="-1603" windowWidth="26301" windowHeight="14305" xr2:uid="{62BF07D9-DBFF-4528-A9A8-7318055715EB}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="39">
   <si>
     <t>positive candidates</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>missing game tape for last 3/4 of 4th quarter</t>
+  </si>
+  <si>
+    <t>total candidates</t>
   </si>
 </sst>
 </file>
@@ -572,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C99D260-17EE-4B29-B6BB-D4F26CA46663}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -610,28 +613,37 @@
     </row>
     <row r="4" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B4">
+        <f>B2+B3</f>
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B4)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="6" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B5)</f>
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6">
-        <f>(B2 - B4)/(B2 - B4 + B5)</f>
+    <row r="7" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <f>(B2 - B5)/(B2 - B5 + B6)</f>
         <v>0.88309636650868883</v>
       </c>
     </row>
@@ -2586,7 +2598,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="b">
-        <f>Overall!B6=(B2 - B4)/(B2 - B4 + B5)</f>
+        <f>Overall!B7=(B2 - B4)/(B2 - B4 + B5)</f>
         <v>0</v>
       </c>
       <c r="D6">

</xml_diff>

<commit_message>
Updated labled data sets to include player_ids
</commit_message>
<xml_diff>
--- a/static/data/notes/CandidateSummaries.xlsx
+++ b/static/data/notes/CandidateSummaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanos\Documents\Dev\NBAThesis\NBA_Thesis\static\data\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406D7350-7AC6-4D75-AF5D-4FD1FB0D2034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D877B3A7-66FF-4703-AE57-AC0E81C815B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26192" yWindow="-1603" windowWidth="26301" windowHeight="14305" xr2:uid="{62BF07D9-DBFF-4528-A9A8-7318055715EB}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{62BF07D9-DBFF-4528-A9A8-7318055715EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <sheet name="20160123LALPOR" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -578,7 +577,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -599,7 +598,7 @@
       </c>
       <c r="B2">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B2)</f>
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -608,7 +607,7 @@
       </c>
       <c r="B3">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B3)</f>
-        <v>1282</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +616,7 @@
       </c>
       <c r="B4">
         <f>B2+B3</f>
-        <v>1876</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -644,7 +643,7 @@
       </c>
       <c r="B7" s="6">
         <f>(B2 - B5)/(B2 - B5 + B6)</f>
-        <v>0.88309636650868883</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
   </sheetData>
@@ -657,7 +656,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -698,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -739,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -803,7 +802,7 @@
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.94736842105263153</v>
+        <v>0.94871794871794868</v>
       </c>
     </row>
   </sheetData>
@@ -1706,7 +1705,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -1794,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1854,7 +1853,7 @@
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.83333333333333337</v>
+        <v>0.82857142857142863</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2064,7 +2063,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2108,7 +2107,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -2215,7 +2214,7 @@
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.7321428571428571</v>
+        <v>0.74137931034482762</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2407,7 +2406,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2495,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2910,7 +2909,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2954,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -2998,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3089,7 +3088,7 @@
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.96969696969696972</v>
+        <v>0.96296296296296291</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -3222,7 +3221,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3310,7 +3309,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D3">
         <v>163</v>
@@ -3509,7 +3508,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3593,7 +3592,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>125</v>
@@ -3736,7 +3735,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -4109,7 +4108,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -4195,7 +4194,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -4317,7 +4316,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -4403,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>

<commit_message>
Final adjustments to models and game process, now working, parsed 5 mil rows into the databse
</commit_message>
<xml_diff>
--- a/static/data/notes/CandidateSummaries.xlsx
+++ b/static/data/notes/CandidateSummaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanos\Documents\Dev\NBAThesis\NBA_Thesis\static\data\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D877B3A7-66FF-4703-AE57-AC0E81C815B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34946CCE-C830-4C86-87FC-FC32BB123668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{62BF07D9-DBFF-4528-A9A8-7318055715EB}"/>
+    <workbookView xWindow="-26192" yWindow="-1603" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="6" xr2:uid="{62BF07D9-DBFF-4528-A9A8-7318055715EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -576,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C99D260-17EE-4B29-B6BB-D4F26CA46663}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -598,7 +598,7 @@
       </c>
       <c r="B2">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B2)</f>
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -607,7 +607,7 @@
       </c>
       <c r="B3">
         <f>SUM('20151106MILNYK:20160123LALPOR'!B3)</f>
-        <v>1322</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -616,7 +616,7 @@
       </c>
       <c r="B4">
         <f>B2+B3</f>
-        <v>1912</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
       </c>
       <c r="B7" s="6">
         <f>(B2 - B5)/(B2 - B5 + B6)</f>
-        <v>0.88235294117647056</v>
+        <v>0.88216560509554143</v>
       </c>
     </row>
   </sheetData>
@@ -3734,8 +3734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065A868-8FBB-4D38-872A-E4D2D60D3BF7}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3778,7 +3778,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -3819,7 +3819,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3">
         <v>40</v>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B6" s="7">
         <f>(B2 - B4)/(B2 - B4 + B5)</f>
-        <v>0.85074626865671643</v>
+        <v>0.84848484848484851</v>
       </c>
       <c r="D6">
         <v>125</v>

</xml_diff>